<commit_message>
fig 5 data and analysis
</commit_message>
<xml_diff>
--- a/synthetic-cell-state-biomarkers.xlsx
+++ b/synthetic-cell-state-biomarkers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aqib/Desktop/BCCL/char-syn-gene-nets/circuit-state/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02AB134-5C98-184C-ADDE-851ED9419225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679D7F02-B17E-F24B-8549-89C3607B0BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11200" yWindow="5900" windowWidth="28800" windowHeight="17500" xr2:uid="{552E05E8-83AF-0E4B-B324-2E62912FB4B6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="157">
   <si>
     <t>gene</t>
   </si>
@@ -947,6 +947,9 @@
     <t>increased sensitivity to g-type lysozyme in the presence of EDTA
 also decreased ability to respire using alpha-ketoglutaric acid or succinic acid
 also decreased g-lysozyme inhibition -&gt; cell death</t>
+  </si>
+  <si>
+    <t>https://ecoliwiki.org/colipedia/index.php/pliG:Gene</t>
   </si>
 </sst>
 </file>
@@ -1374,8 +1377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B39F551-611F-CA48-A6AE-A3F53E814C65}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="134" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1385,7 +1388,7 @@
     <col min="3" max="3" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="41.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" style="1"/>
     <col min="9" max="9" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -1611,6 +1614,9 @@
       </c>
       <c r="E10" s="7" t="s">
         <v>155</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>156</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>82</v>

</xml_diff>